<commit_message>
BX-6366: update UPD generation
</commit_message>
<xml_diff>
--- a/storage/app/document-templates/upd.xlsx
+++ b/storage/app/document-templates/upd.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="125">
   <si>
     <t>Универсальный передаточный документ</t>
   </si>
@@ -65,9 +65,6 @@
     <t xml:space="preserve">    Статус:</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Адрес:</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>1б</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>2а</t>
@@ -620,7 +620,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -651,13 +651,13 @@
     <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="14" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -681,6 +681,9 @@
     <xf borderId="8" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="8" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -701,9 +704,6 @@
     </xf>
     <xf borderId="8" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -1243,16 +1243,16 @@
       <c r="B5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>17</v>
+      <c r="D5" s="15">
+        <v>2.0</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="3"/>
       <c r="G5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>19</v>
       </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -1286,13 +1286,13 @@
       <c r="AV5" s="6"/>
       <c r="AW5" s="6"/>
       <c r="AX5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="AZ5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="BF5" s="11" t="s">
         <v>20</v>
-      </c>
-      <c r="AZ5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="BF5" s="11" t="s">
-        <v>21</v>
       </c>
       <c r="BG5" s="6"/>
       <c r="BH5" s="6"/>
@@ -1308,7 +1308,7 @@
       <c r="BR5" s="6"/>
       <c r="BS5" s="6"/>
       <c r="BT5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="BX5" s="1"/>
     </row>
@@ -1320,10 +1320,10 @@
       <c r="E6" s="1"/>
       <c r="F6" s="3"/>
       <c r="G6" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" s="11" t="s">
         <v>23</v>
-      </c>
-      <c r="R6" s="11" t="s">
-        <v>24</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -1357,13 +1357,13 @@
       <c r="AV6" s="6"/>
       <c r="AW6" s="6"/>
       <c r="AX6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="AZ6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="AZ6" s="16" t="s">
+      <c r="BF6" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="BF6" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="BG6" s="6"/>
       <c r="BH6" s="6"/>
@@ -1379,18 +1379,18 @@
       <c r="BR6" s="6"/>
       <c r="BS6" s="6"/>
       <c r="BT6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="BX6" s="1"/>
     </row>
-    <row r="7" ht="11.25" customHeight="1">
+    <row r="7" ht="16.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="R7" s="11" t="s">
         <v>8</v>
@@ -1427,13 +1427,13 @@
       <c r="AV7" s="6"/>
       <c r="AW7" s="6"/>
       <c r="AX7" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AZ7" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AZ7" s="2" t="s">
+      <c r="BF7" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="BF7" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="BG7" s="6"/>
       <c r="BH7" s="6"/>
@@ -1449,15 +1449,15 @@
       <c r="BR7" s="6"/>
       <c r="BS7" s="6"/>
       <c r="BT7" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="BX7" s="1"/>
     </row>
-    <row r="8" ht="11.25" customHeight="1">
+    <row r="8" ht="16.5" customHeight="1">
       <c r="A8" s="1"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="2" t="s">
-        <v>35</v>
+      <c r="G8" s="16" t="s">
+        <v>34</v>
       </c>
       <c r="R8" s="11" t="s">
         <v>8</v>
@@ -1494,14 +1494,14 @@
       <c r="AV8" s="6"/>
       <c r="AW8" s="6"/>
       <c r="AX8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="AZ8" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="AZ8" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="BL8" s="4"/>
       <c r="BT8" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="BX8" s="1"/>
     </row>
@@ -1509,10 +1509,10 @@
       <c r="A9" s="1"/>
       <c r="F9" s="3"/>
       <c r="G9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="R9" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="R9" s="11" t="s">
-        <v>40</v>
       </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -1546,7 +1546,7 @@
       <c r="AV9" s="6"/>
       <c r="AW9" s="6"/>
       <c r="AX9" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BL9" s="6"/>
       <c r="BM9" s="6"/>
@@ -1562,10 +1562,10 @@
       <c r="A10" s="1"/>
       <c r="F10" s="3"/>
       <c r="G10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R10" s="11" t="s">
         <v>42</v>
-      </c>
-      <c r="R10" s="11" t="s">
-        <v>43</v>
       </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -1599,7 +1599,7 @@
       <c r="AV10" s="6"/>
       <c r="AW10" s="6"/>
       <c r="AX10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="AZ10" s="1"/>
       <c r="BA10" s="1"/>
@@ -1695,19 +1695,19 @@
     </row>
     <row r="12" ht="27.0" customHeight="1">
       <c r="B12" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="21"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
       <c r="F12" s="22" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="21"/>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
       <c r="J12" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12" s="21"/>
@@ -1718,24 +1718,24 @@
       <c r="Q12" s="21"/>
       <c r="R12" s="23"/>
       <c r="S12" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T12" s="21"/>
       <c r="U12" s="21"/>
       <c r="V12" s="23"/>
       <c r="W12" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="X12" s="25"/>
       <c r="Y12" s="25"/>
       <c r="Z12" s="25"/>
       <c r="AA12" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB12" s="21"/>
       <c r="AC12" s="21"/>
       <c r="AD12" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE12" s="21"/>
       <c r="AF12" s="21"/>
@@ -1747,7 +1747,7 @@
       <c r="AL12" s="21"/>
       <c r="AM12" s="21"/>
       <c r="AN12" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AO12" s="21"/>
       <c r="AP12" s="21"/>
@@ -1758,29 +1758,29 @@
       <c r="AU12" s="21"/>
       <c r="AV12" s="21"/>
       <c r="AW12" s="20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AX12" s="21"/>
       <c r="AY12" s="21"/>
       <c r="AZ12" s="21"/>
       <c r="BA12" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="BB12" s="21"/>
       <c r="BC12" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="BD12" s="21"/>
       <c r="BE12" s="21"/>
       <c r="BF12" s="21"/>
       <c r="BG12" s="20" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="BH12" s="21"/>
       <c r="BI12" s="21"/>
       <c r="BJ12" s="23"/>
       <c r="BK12" s="24" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BL12" s="25"/>
       <c r="BM12" s="25"/>
@@ -1789,7 +1789,7 @@
       <c r="BP12" s="25"/>
       <c r="BQ12" s="26"/>
       <c r="BR12" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BS12" s="21"/>
       <c r="BT12" s="21"/>
@@ -1819,11 +1819,11 @@
       <c r="U13" s="6"/>
       <c r="V13" s="29"/>
       <c r="W13" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X13" s="25"/>
       <c r="Y13" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z13" s="25"/>
       <c r="AA13" s="27"/>
@@ -1863,14 +1863,14 @@
       <c r="BI13" s="6"/>
       <c r="BJ13" s="29"/>
       <c r="BK13" s="30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BL13" s="6"/>
       <c r="BM13" s="6"/>
       <c r="BN13" s="6"/>
       <c r="BO13" s="29"/>
       <c r="BP13" s="30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="BQ13" s="29"/>
       <c r="BR13" s="27"/>
@@ -1881,19 +1881,19 @@
     </row>
     <row r="14" ht="11.25" customHeight="1">
       <c r="B14" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="26"/>
       <c r="J14" s="33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K14" s="25"/>
       <c r="L14" s="25"/>
@@ -1904,13 +1904,13 @@
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
       <c r="S14" s="33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
       <c r="V14" s="26"/>
       <c r="W14" s="31" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="X14" s="6"/>
       <c r="Y14" s="31" t="s">
@@ -2028,7 +2028,7 @@
       </c>
       <c r="AB15" s="25"/>
       <c r="AC15" s="26"/>
-      <c r="AD15" s="39" t="s">
+      <c r="AD15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="AE15" s="25"/>
@@ -2057,11 +2057,11 @@
       <c r="AX15" s="25"/>
       <c r="AY15" s="25"/>
       <c r="AZ15" s="26"/>
-      <c r="BA15" s="35" t="s">
+      <c r="BA15" s="41" t="s">
         <v>8</v>
       </c>
       <c r="BB15" s="26"/>
-      <c r="BC15" s="39" t="s">
+      <c r="BC15" s="40" t="s">
         <v>8</v>
       </c>
       <c r="BD15" s="25"/>
@@ -2073,7 +2073,7 @@
       <c r="BH15" s="25"/>
       <c r="BI15" s="25"/>
       <c r="BJ15" s="26"/>
-      <c r="BK15" s="35" t="s">
+      <c r="BK15" s="41" t="s">
         <v>8</v>
       </c>
       <c r="BL15" s="25"/>
@@ -2095,11 +2095,11 @@
       <c r="BX15" s="34"/>
     </row>
     <row r="16" ht="11.25" customHeight="1">
-      <c r="B16" s="41"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="44" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="45" t="s">
         <v>80</v>
       </c>
       <c r="G16" s="6"/>
@@ -2114,18 +2114,18 @@
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="45"/>
-      <c r="AA16" s="45"/>
-      <c r="AB16" s="45"/>
-      <c r="AC16" s="45"/>
-      <c r="AD16" s="45"/>
+      <c r="S16" s="46"/>
+      <c r="T16" s="46"/>
+      <c r="U16" s="46"/>
+      <c r="V16" s="46"/>
+      <c r="W16" s="46"/>
+      <c r="X16" s="46"/>
+      <c r="Y16" s="46"/>
+      <c r="Z16" s="46"/>
+      <c r="AA16" s="46"/>
+      <c r="AB16" s="46"/>
+      <c r="AC16" s="46"/>
+      <c r="AD16" s="46"/>
       <c r="AE16" s="6"/>
       <c r="AF16" s="6"/>
       <c r="AG16" s="6"/>
@@ -2135,7 +2135,7 @@
       <c r="AK16" s="6"/>
       <c r="AL16" s="6"/>
       <c r="AM16" s="6"/>
-      <c r="AN16" s="46">
+      <c r="AN16" s="47">
         <v>360685.59</v>
       </c>
       <c r="AO16" s="25"/>
@@ -2146,7 +2146,7 @@
       <c r="AT16" s="25"/>
       <c r="AU16" s="25"/>
       <c r="AV16" s="26"/>
-      <c r="AW16" s="47" t="s">
+      <c r="AW16" s="48" t="s">
         <v>81</v>
       </c>
       <c r="AX16" s="25"/>
@@ -2154,19 +2154,19 @@
       <c r="AZ16" s="25"/>
       <c r="BA16" s="25"/>
       <c r="BB16" s="26"/>
-      <c r="BC16" s="48" t="s">
+      <c r="BC16" s="47" t="s">
         <v>8</v>
       </c>
       <c r="BD16" s="25"/>
       <c r="BE16" s="25"/>
       <c r="BF16" s="26"/>
-      <c r="BG16" s="46">
+      <c r="BG16" s="47">
         <v>360685.59</v>
       </c>
       <c r="BH16" s="25"/>
       <c r="BI16" s="25"/>
       <c r="BJ16" s="26"/>
-      <c r="BK16" s="41"/>
+      <c r="BK16" s="42"/>
       <c r="BL16" s="25"/>
       <c r="BM16" s="25"/>
       <c r="BN16" s="25"/>

</xml_diff>